<commit_message>
perbaikan data sample excel
</commit_message>
<xml_diff>
--- a/format_bank.xlsx
+++ b/format_bank.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\musti\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ardiandp\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="33">
   <si>
     <t>Tanggal</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t xml:space="preserve">TRSF E-BANKING CR 04/30 95031 JAN FENY PHILLIP HANDOKO </t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -462,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -474,11 +477,11 @@
     <col min="2" max="2" width="62.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.42578125"/>
     <col min="4" max="4" width="19.7109375"/>
-    <col min="5" max="5" width="44.42578125"/>
-    <col min="6" max="1025" width="11.5703125"/>
+    <col min="6" max="6" width="44.42578125"/>
+    <col min="7" max="1026" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -492,10 +495,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -508,11 +514,12 @@
       <c r="D2" s="2">
         <v>2800000</v>
       </c>
-      <c r="E2" s="2">
-        <v>243176207</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2">
+        <v>243176207</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -525,14 +532,15 @@
       <c r="D3" s="2">
         <v>2800000</v>
       </c>
-      <c r="E3" s="2">
-        <v>243176207</v>
-      </c>
-      <c r="F3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E3" s="2"/>
+      <c r="F3" s="2">
+        <v>243176207</v>
+      </c>
+      <c r="G3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -545,11 +553,12 @@
       <c r="D4" s="2">
         <v>2800000</v>
       </c>
-      <c r="E4" s="2">
-        <v>243176207</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2">
+        <v>243176207</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -562,11 +571,12 @@
       <c r="D5" s="2">
         <v>2800000</v>
       </c>
-      <c r="E5" s="2">
-        <v>243176207</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E5" s="2"/>
+      <c r="F5" s="2">
+        <v>243176207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -579,11 +589,12 @@
       <c r="D6" s="2">
         <v>2800000</v>
       </c>
-      <c r="E6" s="2">
-        <v>243176207</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2">
+        <v>243176207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -596,11 +607,12 @@
       <c r="D7" s="2">
         <v>2800000</v>
       </c>
-      <c r="E7" s="2">
-        <v>243176207</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2">
+        <v>243176207</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -613,11 +625,12 @@
       <c r="D8" s="2">
         <v>2800000</v>
       </c>
-      <c r="E8" s="2">
-        <v>243176207</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E8" s="2"/>
+      <c r="F8" s="2">
+        <v>243176207</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -630,11 +643,12 @@
       <c r="D9" s="2">
         <v>2800000</v>
       </c>
-      <c r="E9" s="2">
-        <v>243176207</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E9" s="2"/>
+      <c r="F9" s="2">
+        <v>243176207</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -647,11 +661,12 @@
       <c r="D10" s="2">
         <v>2800000</v>
       </c>
-      <c r="E10" s="2">
-        <v>243176207</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E10" s="2"/>
+      <c r="F10" s="2">
+        <v>243176207</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -664,11 +679,12 @@
       <c r="D11" s="2">
         <v>2800000</v>
       </c>
-      <c r="E11" s="2">
-        <v>243176207</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E11" s="2"/>
+      <c r="F11" s="2">
+        <v>243176207</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -681,11 +697,12 @@
       <c r="D12" s="2">
         <v>2800000</v>
       </c>
-      <c r="E12" s="2">
-        <v>243176207</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E12" s="2"/>
+      <c r="F12" s="2">
+        <v>243176207</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -698,11 +715,12 @@
       <c r="D13" s="2">
         <v>2800000</v>
       </c>
-      <c r="E13" s="2">
-        <v>243176207</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E13" s="2"/>
+      <c r="F13" s="2">
+        <v>243176207</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -715,11 +733,12 @@
       <c r="D14" s="2">
         <v>2800000</v>
       </c>
-      <c r="E14" s="2">
-        <v>243176207</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E14" s="2"/>
+      <c r="F14" s="2">
+        <v>243176207</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -732,11 +751,12 @@
       <c r="D15" s="2">
         <v>2800000</v>
       </c>
-      <c r="E15" s="2">
-        <v>243176207</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E15" s="2"/>
+      <c r="F15" s="2">
+        <v>243176207</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -749,11 +769,12 @@
       <c r="D16" s="2">
         <v>2800000</v>
       </c>
-      <c r="E16" s="2">
-        <v>243176207</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E16" s="2"/>
+      <c r="F16" s="2">
+        <v>243176207</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -766,11 +787,12 @@
       <c r="D17" s="2">
         <v>2800000</v>
       </c>
-      <c r="E17" s="2">
-        <v>243176207</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E17" s="2"/>
+      <c r="F17" s="2">
+        <v>243176207</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -783,11 +805,12 @@
       <c r="D18" s="2">
         <v>2800000</v>
       </c>
-      <c r="E18" s="2">
-        <v>243176207</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E18" s="2"/>
+      <c r="F18" s="2">
+        <v>243176207</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -800,11 +823,12 @@
       <c r="D19" s="2">
         <v>2800000</v>
       </c>
-      <c r="E19" s="2">
-        <v>243176207</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E19" s="2"/>
+      <c r="F19" s="2">
+        <v>243176207</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -817,11 +841,12 @@
       <c r="D20" s="2">
         <v>2800000</v>
       </c>
-      <c r="E20" s="2">
-        <v>243176207</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E20" s="2"/>
+      <c r="F20" s="2">
+        <v>243176207</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -834,11 +859,12 @@
       <c r="D21" s="2">
         <v>2800000</v>
       </c>
-      <c r="E21" s="2">
-        <v>243176207</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E21" s="2"/>
+      <c r="F21" s="2">
+        <v>243176207</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -851,11 +877,12 @@
       <c r="D22" s="2">
         <v>2800000</v>
       </c>
-      <c r="E22" s="2">
-        <v>243176207</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E22" s="2"/>
+      <c r="F22" s="2">
+        <v>243176207</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -868,11 +895,12 @@
       <c r="D23" s="2">
         <v>2800000</v>
       </c>
-      <c r="E23" s="2">
-        <v>243176207</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E23" s="2"/>
+      <c r="F23" s="2">
+        <v>243176207</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -885,11 +913,12 @@
       <c r="D24" s="2">
         <v>2800000</v>
       </c>
-      <c r="E24" s="2">
-        <v>243176207</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E24" s="2"/>
+      <c r="F24" s="2">
+        <v>243176207</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -902,11 +931,12 @@
       <c r="D25" s="2">
         <v>2800000</v>
       </c>
-      <c r="E25" s="2">
-        <v>243176207</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E25" s="2"/>
+      <c r="F25" s="2">
+        <v>243176207</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -919,7 +949,8 @@
       <c r="D26" s="2">
         <v>2800000</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="2"/>
+      <c r="F26" s="2">
         <v>243176207</v>
       </c>
     </row>

</xml_diff>